<commit_message>
update manuscript and tables
</commit_message>
<xml_diff>
--- a/tables/table_aorta_univariate.xlsx
+++ b/tables/table_aorta_univariate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\md1spsx\Documents\PaperRifampicin\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\md1spsx\Documents\GitHub\tristan-paper-first-in-human\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3424BF88-2695-4229-B44B-954B1B767421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70425A8D-F21C-4799-A281-63004F23DA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1824" yWindow="552" windowWidth="18768" windowHeight="8604" xr2:uid="{2C6F02DA-1317-44C6-82D9-DCA3D83633FA}"/>
+    <workbookView xWindow="11220" yWindow="900" windowWidth="11844" windowHeight="9492" xr2:uid="{2C6F02DA-1317-44C6-82D9-DCA3D83633FA}"/>
   </bookViews>
   <sheets>
     <sheet name="table_aorta_univariate" sheetId="1" r:id="rId1"/>
@@ -28,87 +28,9 @@
     <t>Effect (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">28 (6.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.7 (2.6) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.3 (3.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.3 (2.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">46 (9.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (2.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 (4.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (6.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.2 (1.5) </t>
-  </si>
-  <si>
     <t xml:space="preserve">35 (8.0) </t>
   </si>
   <si>
-    <t xml:space="preserve">18 (7.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.0 (1.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (2.8) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (3.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (7.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.4 (1.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.4 (0.8) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">49 (11) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 (18) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-41 (17) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 (25) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.4 (20) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.7 (19) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-23 (10) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.3 (17) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.8 (25) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">230 (330) </t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -143,6 +65,84 @@
   </si>
   <si>
     <t>MTT (o, e) - Organs extravascular mean transit time (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 (16) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (16) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 (8.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (7.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">136 (130) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.7 (2.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.7 (1.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (27) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.7 (2.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5 (0.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-41 (16) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (3.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (2.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 (23) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 (8.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 (8.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 (9.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (3.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (3.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25 (12) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 (5.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (7.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.7 (20) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.0 (1.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.7 (1.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (48) </t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1255,13 +1255,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -1272,16 +1272,16 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" s="12">
         <v>0.01</v>
@@ -1289,50 +1289,50 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E3" s="13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="12">
-        <v>0.27</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" s="13">
         <v>0.02</v>
@@ -1340,87 +1340,87 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6" s="12">
-        <v>0.47</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E7" s="13">
-        <v>0.61</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E8" s="14">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E9" s="13">
-        <v>0.85</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="16">
-        <v>0.85</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>